<commit_message>
Refactor config, docker, and deployment. Open to adding supporting services
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1035FE0B-9828-CA4C-87D7-0008EA506364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FEEB56-EF82-524F-9226-3091BF8668AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="24460" windowHeight="14900" xr2:uid="{21C299CA-AAA5-994F-A29D-AE16A83D7C73}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="24460" windowHeight="14900" activeTab="2" xr2:uid="{21C299CA-AAA5-994F-A29D-AE16A83D7C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="304">
   <si>
     <t>gRPC testing checklist</t>
   </si>
@@ -1013,6 +1013,9 @@
   </si>
   <si>
     <t>* most literal values recorded, plus message types, are defined in the corresponding .proto files associated with the test</t>
+  </si>
+  <si>
+    <t>* all tests, unless mentioned otherwise, are performed with gRPC</t>
   </si>
 </sst>
 </file>
@@ -1166,26 +1169,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,15 +1187,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1566,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A23E273-8971-684D-B228-C19739A81024}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,18 +1609,18 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="13" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="13" t="s">
         <v>289</v>
       </c>
     </row>
@@ -1688,6 +1691,11 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -1703,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21BFCB4-0742-3441-8DBF-D8558B20D680}">
   <dimension ref="A1:BF166"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="C84" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1741,90 +1749,90 @@
       <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:58" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="18" t="s">
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18" t="s">
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18" t="s">
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="18"/>
-      <c r="AI4" s="18" t="s">
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AJ4" s="18"/>
-      <c r="AK4" s="18"/>
-      <c r="AL4" s="18"/>
-      <c r="AM4" s="18"/>
-      <c r="AN4" s="18"/>
-      <c r="AO4" s="18" t="s">
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AP4" s="18"/>
-      <c r="AQ4" s="18"/>
-      <c r="AR4" s="18"/>
-      <c r="AS4" s="18"/>
-      <c r="AT4" s="18"/>
-      <c r="AU4" s="19" t="s">
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17"/>
+      <c r="AU4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AV4" s="19"/>
-      <c r="AW4" s="19"/>
-      <c r="AX4" s="19"/>
-      <c r="AY4" s="19"/>
-      <c r="AZ4" s="19"/>
-      <c r="BA4" s="18"/>
-      <c r="BB4" s="18"/>
-      <c r="BC4" s="18"/>
-      <c r="BD4" s="18"/>
-      <c r="BE4" s="18"/>
-      <c r="BF4" s="18"/>
+      <c r="AV4" s="18"/>
+      <c r="AW4" s="18"/>
+      <c r="AX4" s="18"/>
+      <c r="AY4" s="18"/>
+      <c r="AZ4" s="18"/>
+      <c r="BA4" s="17"/>
+      <c r="BB4" s="17"/>
+      <c r="BC4" s="17"/>
+      <c r="BD4" s="17"/>
+      <c r="BE4" s="17"/>
+      <c r="BF4" s="17"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3209,18 +3217,18 @@
       <c r="AT15" t="s">
         <v>30</v>
       </c>
-      <c r="AU15" s="11" t="s">
+      <c r="AU15" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="AV15" s="11"/>
-      <c r="AW15" s="11"/>
-      <c r="AX15" s="11"/>
-      <c r="AY15" s="11"/>
-      <c r="AZ15" s="11"/>
-      <c r="BA15" s="11"/>
-      <c r="BB15" s="11"/>
-      <c r="BC15" s="11"/>
-      <c r="BD15" s="11"/>
+      <c r="AV15" s="16"/>
+      <c r="AW15" s="16"/>
+      <c r="AX15" s="16"/>
+      <c r="AY15" s="16"/>
+      <c r="AZ15" s="16"/>
+      <c r="BA15" s="16"/>
+      <c r="BB15" s="16"/>
+      <c r="BC15" s="16"/>
+      <c r="BD15" s="16"/>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3340,13 +3348,13 @@
       <c r="AU16" t="s">
         <v>191</v>
       </c>
-      <c r="AV16" s="11" t="s">
+      <c r="AV16" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="AW16" s="11"/>
-      <c r="AX16" s="11"/>
-      <c r="AY16" s="11"/>
-      <c r="AZ16" s="11"/>
+      <c r="AW16" s="16"/>
+      <c r="AX16" s="16"/>
+      <c r="AY16" s="16"/>
+      <c r="AZ16" s="16"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -3919,50 +3927,50 @@
       </c>
     </row>
     <row r="35" spans="1:40" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12" t="s">
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="R35" s="12"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="12"/>
-      <c r="U35" s="12"/>
-      <c r="V35" s="12"/>
-      <c r="W35" s="12"/>
-      <c r="X35" s="12"/>
-      <c r="Y35" s="12"/>
-      <c r="Z35" s="12"/>
-      <c r="AA35" s="12"/>
-      <c r="AB35" s="12"/>
-      <c r="AC35" s="12" t="s">
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="19"/>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AD35" s="12"/>
-      <c r="AE35" s="12"/>
-      <c r="AF35" s="12"/>
-      <c r="AG35" s="12"/>
-      <c r="AH35" s="12"/>
-      <c r="AI35" s="12" t="s">
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="19"/>
+      <c r="AF35" s="19"/>
+      <c r="AG35" s="19"/>
+      <c r="AH35" s="19"/>
+      <c r="AI35" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="AJ35" s="12"/>
-      <c r="AK35" s="12"/>
-      <c r="AL35" s="12"/>
-      <c r="AM35" s="12"/>
-      <c r="AN35" s="12"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
+      <c r="AL35" s="19"/>
+      <c r="AM35" s="19"/>
+      <c r="AN35" s="19"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -5818,19 +5826,19 @@
       <c r="G67" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="16"/>
-      <c r="O67" s="16"/>
-      <c r="P67" s="16"/>
-      <c r="Q67" s="16"/>
-      <c r="R67" s="16"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="23"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="23"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="23"/>
     </row>
     <row r="68" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
@@ -5908,14 +5916,14 @@
       <c r="K74" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L74" s="16" t="s">
+      <c r="L74" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="M74" s="16"/>
-      <c r="N74" s="16"/>
-      <c r="O74" s="16"/>
-      <c r="P74" s="16"/>
-      <c r="Q74" s="16"/>
+      <c r="M74" s="23"/>
+      <c r="N74" s="23"/>
+      <c r="O74" s="23"/>
+      <c r="P74" s="23"/>
+      <c r="Q74" s="23"/>
       <c r="R74" s="4"/>
     </row>
     <row r="75" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6122,30 +6130,30 @@
       <c r="B90" t="s">
         <v>177</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13" t="s">
+      <c r="D90" s="24"/>
+      <c r="E90" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13" t="s">
+      <c r="F90" s="24"/>
+      <c r="G90" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13" t="s">
+      <c r="H90" s="24"/>
+      <c r="I90" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13" t="s">
+      <c r="J90" s="24"/>
+      <c r="K90" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13" t="s">
+      <c r="L90" s="24"/>
+      <c r="M90" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="N90" s="13"/>
+      <c r="N90" s="24"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
@@ -6189,103 +6197,103 @@
       </c>
     </row>
     <row r="92" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="15" t="s">
+      <c r="A92" s="21" t="s">
         <v>165</v>
       </c>
       <c r="B92" t="s">
         <v>166</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D92" s="11"/>
-      <c r="E92" s="14" t="s">
+      <c r="D92" s="16"/>
+      <c r="E92" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="F92" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G92" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H92" s="11" t="s">
+      <c r="H92" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="I92" s="11" t="s">
+      <c r="I92" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="J92" s="11" t="s">
+      <c r="J92" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="K92" s="11" t="s">
+      <c r="K92" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="L92" s="11" t="s">
+      <c r="L92" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="M92" s="11" t="s">
+      <c r="M92" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="N92" s="11" t="s">
+      <c r="N92" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="15"/>
+      <c r="A93" s="21"/>
       <c r="B93" t="s">
         <v>167</v>
       </c>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="11"/>
-      <c r="M93" s="14"/>
-      <c r="N93" s="11"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="16"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="16"/>
     </row>
     <row r="94" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="15"/>
+      <c r="A94" s="21"/>
       <c r="B94" t="s">
         <v>168</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="14"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="14"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="14"/>
-      <c r="N94" s="11"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="16"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="16"/>
+      <c r="M94" s="22"/>
+      <c r="N94" s="16"/>
     </row>
     <row r="95" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="15"/>
+      <c r="A95" s="21"/>
       <c r="B95" t="s">
         <v>169</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="14"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="14"/>
-      <c r="L95" s="11"/>
-      <c r="M95" s="14"/>
-      <c r="N95" s="11"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="16"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="16"/>
+      <c r="M95" s="22"/>
+      <c r="N95" s="16"/>
     </row>
     <row r="96" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="21" t="s">
         <v>172</v>
       </c>
       <c r="B96" t="s">
@@ -6329,7 +6337,7 @@
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A97" s="15"/>
+      <c r="A97" s="21"/>
       <c r="B97" t="s">
         <v>167</v>
       </c>
@@ -6371,7 +6379,7 @@
       </c>
     </row>
     <row r="98" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A98" s="15"/>
+      <c r="A98" s="21"/>
       <c r="B98" t="s">
         <v>168</v>
       </c>
@@ -6413,7 +6421,7 @@
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A99" s="15"/>
+      <c r="A99" s="21"/>
       <c r="B99" t="s">
         <v>169</v>
       </c>
@@ -6497,13 +6505,13 @@
       <c r="I115" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J115" s="11" t="s">
+      <c r="J115" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="K115" s="11"/>
-      <c r="L115" s="11"/>
-      <c r="M115" s="11"/>
-      <c r="N115" s="11"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
+      <c r="M115" s="16"/>
+      <c r="N115" s="16"/>
     </row>
     <row r="116" spans="1:15" ht="52" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
@@ -7507,21 +7515,21 @@
       <c r="D156" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E156" s="11" t="s">
+      <c r="E156" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="F156" s="11"/>
-      <c r="G156" s="11"/>
-      <c r="H156" s="11"/>
+      <c r="F156" s="16"/>
+      <c r="G156" s="16"/>
+      <c r="H156" s="16"/>
       <c r="I156" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="J156" s="11" t="s">
+      <c r="J156" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="K156" s="11"/>
-      <c r="L156" s="11"/>
-      <c r="M156" s="11"/>
+      <c r="K156" s="16"/>
+      <c r="L156" s="16"/>
+      <c r="M156" s="16"/>
       <c r="N156" s="4"/>
       <c r="O156" s="4"/>
     </row>
@@ -7572,22 +7580,22 @@
       <c r="B159" t="s">
         <v>270</v>
       </c>
-      <c r="C159" s="21" t="s">
+      <c r="C159" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D159" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E159" s="21" t="s">
+      <c r="D159" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E159" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F159" s="22" t="s">
+      <c r="F159" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="G159" s="21" t="s">
+      <c r="G159" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H159" s="22" t="s">
+      <c r="H159" s="12" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7598,165 +7606,135 @@
       <c r="B160" t="s">
         <v>270</v>
       </c>
-      <c r="C160" s="21"/>
-      <c r="D160" s="21" t="s">
+      <c r="C160" s="11"/>
+      <c r="D160" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E160" s="21"/>
-      <c r="F160" s="21" t="s">
+      <c r="E160" s="11"/>
+      <c r="F160" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G160" s="21"/>
-      <c r="H160" s="21" t="s">
+      <c r="G160" s="11"/>
+      <c r="H160" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="20" t="s">
+      <c r="A161" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B161" t="s">
         <v>271</v>
       </c>
-      <c r="C161" s="21" t="s">
+      <c r="C161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D161" s="21"/>
-      <c r="E161" s="21" t="s">
+      <c r="D161" s="11"/>
+      <c r="E161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F161" s="21"/>
-      <c r="G161" s="21" t="s">
+      <c r="F161" s="11"/>
+      <c r="G161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H161" s="21"/>
+      <c r="H161" s="11"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A162" s="20"/>
+      <c r="A162" s="15"/>
       <c r="B162" t="s">
         <v>270</v>
       </c>
-      <c r="C162" s="21" t="s">
+      <c r="C162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D162" s="21"/>
-      <c r="E162" s="21" t="s">
+      <c r="D162" s="11"/>
+      <c r="E162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F162" s="21"/>
-      <c r="G162" s="21" t="s">
+      <c r="F162" s="11"/>
+      <c r="G162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H162" s="21"/>
+      <c r="H162" s="11"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" s="20" t="s">
+      <c r="A163" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B163" t="s">
         <v>271</v>
       </c>
-      <c r="C163" s="21" t="s">
+      <c r="C163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D163" s="21"/>
-      <c r="E163" s="21" t="s">
+      <c r="D163" s="11"/>
+      <c r="E163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F163" s="21"/>
-      <c r="G163" s="21" t="s">
+      <c r="F163" s="11"/>
+      <c r="G163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H163" s="21"/>
+      <c r="H163" s="11"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A164" s="20"/>
+      <c r="A164" s="15"/>
       <c r="B164" t="s">
         <v>270</v>
       </c>
-      <c r="C164" s="21" t="s">
+      <c r="C164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D164" s="21"/>
-      <c r="E164" s="21" t="s">
+      <c r="D164" s="11"/>
+      <c r="E164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F164" s="21"/>
-      <c r="G164" s="21" t="s">
+      <c r="F164" s="11"/>
+      <c r="G164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H164" s="21"/>
+      <c r="H164" s="11"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A165" s="20" t="s">
+      <c r="A165" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B165" t="s">
         <v>271</v>
       </c>
-      <c r="C165" s="21"/>
-      <c r="D165" s="21" t="s">
+      <c r="C165" s="11"/>
+      <c r="D165" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E165" s="21"/>
-      <c r="F165" s="21" t="s">
+      <c r="E165" s="11"/>
+      <c r="F165" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G165" s="21"/>
-      <c r="H165" s="21" t="s">
+      <c r="G165" s="11"/>
+      <c r="H165" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A166" s="20"/>
+      <c r="A166" s="15"/>
       <c r="B166" t="s">
         <v>270</v>
       </c>
-      <c r="C166" s="21"/>
-      <c r="D166" s="21" t="s">
+      <c r="C166" s="11"/>
+      <c r="D166" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E166" s="21"/>
-      <c r="F166" s="21" t="s">
+      <c r="E166" s="11"/>
+      <c r="F166" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G166" s="21"/>
-      <c r="H166" s="21" t="s">
+      <c r="G166" s="11"/>
+      <c r="H166" s="11" t="s">
         <v>175</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="A165:A166"/>
-    <mergeCell ref="E156:H156"/>
-    <mergeCell ref="J156:M156"/>
-    <mergeCell ref="AO4:AT4"/>
-    <mergeCell ref="AU4:AZ4"/>
-    <mergeCell ref="BA4:BF4"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="AC4:AH4"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="E35:P35"/>
-    <mergeCell ref="Q35:AB35"/>
-    <mergeCell ref="AC35:AH35"/>
-    <mergeCell ref="AI4:AN4"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="H67:R67"/>
-    <mergeCell ref="L74:Q74"/>
-    <mergeCell ref="H92:H95"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="C92:D95"/>
-    <mergeCell ref="G92:G95"/>
-    <mergeCell ref="F92:F95"/>
     <mergeCell ref="AV16:AZ16"/>
     <mergeCell ref="J115:N115"/>
     <mergeCell ref="AU15:BD15"/>
@@ -7770,6 +7748,36 @@
     <mergeCell ref="M92:M95"/>
     <mergeCell ref="I92:I95"/>
     <mergeCell ref="K92:K95"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="H67:R67"/>
+    <mergeCell ref="L74:Q74"/>
+    <mergeCell ref="H92:H95"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="C92:D95"/>
+    <mergeCell ref="G92:G95"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="E35:P35"/>
+    <mergeCell ref="Q35:AB35"/>
+    <mergeCell ref="AC35:AH35"/>
+    <mergeCell ref="AI4:AN4"/>
+    <mergeCell ref="AO4:AT4"/>
+    <mergeCell ref="AU4:AZ4"/>
+    <mergeCell ref="BA4:BF4"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="AC4:AH4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="A165:A166"/>
+    <mergeCell ref="E156:H156"/>
+    <mergeCell ref="J156:M156"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7781,8 +7789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA9785-6439-EE40-BF54-969898A6E922}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7810,11 +7818,11 @@
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
       <c r="F2" t="s">
         <v>75</v>
       </c>
@@ -7964,11 +7972,11 @@
       <c r="B9" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" t="s">
         <v>225</v>
       </c>

</xml_diff>

<commit_message>
Fix bugs of compression
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FEEB56-EF82-524F-9226-3091BF8668AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE13A811-5B85-D54D-BD00-2386FD332912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="24460" windowHeight="14900" activeTab="2" xr2:uid="{21C299CA-AAA5-994F-A29D-AE16A83D7C73}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="24460" windowHeight="14900" activeTab="1" xr2:uid="{21C299CA-AAA5-994F-A29D-AE16A83D7C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="311">
   <si>
     <t>gRPC testing checklist</t>
   </si>
@@ -943,9 +943,6 @@
     <t>deflate, gzip</t>
   </si>
   <si>
-    <t>OK, but there is no grpc-accept-encoding and grpc-encoding header from client?</t>
-  </si>
-  <si>
     <t>Welcome to gRPC auto testing record!</t>
   </si>
   <si>
@@ -1016,6 +1013,30 @@
   </si>
   <si>
     <t>* all tests, unless mentioned otherwise, are performed with gRPC</t>
+  </si>
+  <si>
+    <t>Failed: can't find decompressor for deflate</t>
+  </si>
+  <si>
+    <t>Failed: can't find decompressor for deflate (received 4 status headers)</t>
+  </si>
+  <si>
+    <t>Failed: can't find decompressor for deflate (received 4 status headers, but request sent not compressed)</t>
+  </si>
+  <si>
+    <t>Header shows deflate, but message not compressed?</t>
+  </si>
+  <si>
+    <t>Header shows gzip, but message not compressed?</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>java-client: see how decompressor not found error is thrown. Message body not compressed, why not try decompressing?</t>
+  </si>
+  <si>
+    <t>py-client and py-server: see how message compression is coded</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1143,13 +1164,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
@@ -1205,6 +1237,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1583,69 +1616,69 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
         <v>282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" t="s">
         <v>284</v>
-      </c>
-      <c r="B5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>288</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B8" t="s">
         <v>290</v>
-      </c>
-      <c r="B8" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" t="s">
         <v>292</v>
-      </c>
-      <c r="B9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1661,7 +1694,7 @@
         <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1669,33 +1702,33 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B17" t="s">
         <v>297</v>
-      </c>
-      <c r="B17" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" t="s">
         <v>299</v>
-      </c>
-      <c r="B18" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -1709,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21BFCB4-0742-3441-8DBF-D8558B20D680}">
-  <dimension ref="A1:BF166"/>
+  <dimension ref="A1:BF169"/>
   <sheetViews>
-    <sheetView topLeftCell="C84" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92:G95"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7569,11 +7602,20 @@
       <c r="D158" t="s">
         <v>270</v>
       </c>
+      <c r="E158" t="s">
+        <v>278</v>
+      </c>
       <c r="F158" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="G158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H158" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>95</v>
       </c>
@@ -7590,13 +7632,13 @@
         <v>175</v>
       </c>
       <c r="F159" s="12" t="s">
-        <v>279</v>
+        <v>30</v>
       </c>
       <c r="G159" s="11" t="s">
         <v>175</v>
       </c>
       <c r="H159" s="12" t="s">
-        <v>279</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.2">
@@ -7606,20 +7648,26 @@
       <c r="B160" t="s">
         <v>270</v>
       </c>
-      <c r="C160" s="11"/>
+      <c r="C160" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D160" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E160" s="11"/>
+      <c r="E160" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F160" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G160" s="11"/>
+      <c r="G160" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H160" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="15" t="s">
         <v>99</v>
       </c>
@@ -7629,17 +7677,23 @@
       <c r="C161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D161" s="11"/>
+      <c r="D161" s="11" t="s">
+        <v>304</v>
+      </c>
       <c r="E161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F161" s="11"/>
+      <c r="F161" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="G161" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H161" s="11"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H161" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="15"/>
       <c r="B162" t="s">
         <v>270</v>
@@ -7647,17 +7701,23 @@
       <c r="C162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D162" s="11"/>
+      <c r="D162" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="E162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F162" s="11"/>
+      <c r="F162" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="G162" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H162" s="11"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H162" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="15" t="s">
         <v>97</v>
       </c>
@@ -7667,17 +7727,26 @@
       <c r="C163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D163" s="11"/>
+      <c r="D163" s="11" t="s">
+        <v>305</v>
+      </c>
       <c r="E163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F163" s="11"/>
+      <c r="F163" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="G163" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H163" s="11"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H163" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I163" s="25" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="15"/>
       <c r="B164" t="s">
         <v>270</v>
@@ -7685,52 +7754,92 @@
       <c r="C164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D164" s="11"/>
+      <c r="D164" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="E164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F164" s="11"/>
+      <c r="F164" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="G164" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H164" s="11"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H164" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I164" s="25" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B165" t="s">
         <v>271</v>
       </c>
-      <c r="C165" s="11"/>
+      <c r="C165" s="11" t="s">
+        <v>303</v>
+      </c>
       <c r="D165" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E165" s="11"/>
+      <c r="E165" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F165" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G165" s="11"/>
+      <c r="G165" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H165" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I165" s="25" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" t="s">
         <v>270</v>
       </c>
-      <c r="C166" s="11"/>
+      <c r="C166" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D166" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E166" s="11"/>
+      <c r="E166" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F166" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="G166" s="11"/>
+      <c r="G166" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H166" s="11" t="s">
         <v>175</v>
+      </c>
+      <c r="I166" s="25" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>308</v>
+      </c>
+      <c r="B168" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -7789,7 +7898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA9785-6439-EE40-BF54-969898A6E922}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>